<commit_message>
Added more test cases pickup phone order, Dispatch & Proposal
</commit_message>
<xml_diff>
--- a/testData/Hana_T85.xlsx
+++ b/testData/Hana_T85.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DC43BB-F23C-4173-A327-1CF085C8E541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A36DAE2-65F1-4F64-81B0-42754F04C388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1200" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>customername</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>searchandselectcust</t>
-  </si>
-  <si>
-    <t>Abish David 114 N CHURCH ST PICK UP (9566550756,9566550756)</t>
   </si>
 </sst>
 </file>
@@ -97,11 +94,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,14 +405,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -434,11 +430,11 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>